<commit_message>
upgrade of segmentation report file
</commit_message>
<xml_diff>
--- a/doc/Segmentation Test Report.xlsx
+++ b/doc/Segmentation Test Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovannirapa/Documents/GitHub/speech_privacy_android_accelerometer/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39392\Documents\GitHub\speech_privacy_android_accelerometer\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB8237F-57B9-504F-A5EC-56E6F29F9074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32D3A71-A92D-4A60-98AB-153C916B2958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14020" yWindow="4280" windowWidth="19420" windowHeight="10420" xr2:uid="{449DE670-0F7F-4D85-9FF1-3C3B2473E6CE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{449DE670-0F7F-4D85-9FF1-3C3B2473E6CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="111">
   <si>
     <t>Test N°</t>
   </si>
@@ -361,6 +361,12 @@
   </si>
   <si>
     <t>72h</t>
+  </si>
+  <si>
+    <t>7 gg</t>
+  </si>
+  <si>
+    <t>27</t>
   </si>
 </sst>
 </file>
@@ -1131,24 +1137,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EC6811-F8AE-408F-83C6-7E73C05E3EDD}">
   <dimension ref="A1:K162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="107" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="107" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="19" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="37"/>
+    <col min="1" max="3" width="16.36328125" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" customWidth="1"/>
+    <col min="6" max="6" width="10.36328125" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" customWidth="1"/>
+    <col min="8" max="8" width="11.36328125" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" customWidth="1"/>
+    <col min="10" max="10" width="11.6328125" style="19" customWidth="1"/>
+    <col min="11" max="11" width="8.6328125" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1183,7 +1189,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>8</v>
       </c>
@@ -1214,7 +1220,7 @@
       <c r="J2" s="22"/>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>9</v>
       </c>
@@ -1245,7 +1251,7 @@
       <c r="J3" s="20"/>
       <c r="K3" s="33"/>
     </row>
-    <row r="4" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>10</v>
       </c>
@@ -1276,7 +1282,7 @@
       <c r="J4" s="20"/>
       <c r="K4" s="33"/>
     </row>
-    <row r="5" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
         <v>11</v>
       </c>
@@ -1307,7 +1313,7 @@
       <c r="J5" s="20"/>
       <c r="K5" s="33"/>
     </row>
-    <row r="6" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
         <v>12</v>
       </c>
@@ -1338,7 +1344,7 @@
       <c r="J6" s="20"/>
       <c r="K6" s="33"/>
     </row>
-    <row r="7" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
@@ -1369,7 +1375,7 @@
       <c r="J7" s="20"/>
       <c r="K7" s="33"/>
     </row>
-    <row r="8" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
@@ -1400,7 +1406,7 @@
       <c r="J8" s="20"/>
       <c r="K8" s="33"/>
     </row>
-    <row r="9" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
@@ -1431,7 +1437,7 @@
       <c r="J9" s="20"/>
       <c r="K9" s="33"/>
     </row>
-    <row r="10" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
         <v>16</v>
       </c>
@@ -1462,7 +1468,7 @@
       <c r="J10" s="20"/>
       <c r="K10" s="33"/>
     </row>
-    <row r="11" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
         <v>17</v>
       </c>
@@ -1493,7 +1499,7 @@
       <c r="J11" s="20"/>
       <c r="K11" s="33"/>
     </row>
-    <row r="12" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="16" t="s">
         <v>24</v>
       </c>
@@ -1524,7 +1530,7 @@
       <c r="J12" s="25"/>
       <c r="K12" s="34"/>
     </row>
-    <row r="13" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="26" t="s">
         <v>26</v>
       </c>
@@ -1557,7 +1563,7 @@
       </c>
       <c r="K13" s="35"/>
     </row>
-    <row r="14" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>8</v>
       </c>
@@ -1590,7 +1596,7 @@
       </c>
       <c r="K14" s="32"/>
     </row>
-    <row r="15" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>9</v>
       </c>
@@ -1623,7 +1629,7 @@
       </c>
       <c r="K15" s="33"/>
     </row>
-    <row r="16" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>10</v>
       </c>
@@ -1656,7 +1662,7 @@
       </c>
       <c r="K16" s="33"/>
     </row>
-    <row r="17" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>11</v>
       </c>
@@ -1689,7 +1695,7 @@
       </c>
       <c r="K17" s="33"/>
     </row>
-    <row r="18" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
         <v>12</v>
       </c>
@@ -1722,7 +1728,7 @@
       </c>
       <c r="K18" s="33"/>
     </row>
-    <row r="19" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>13</v>
       </c>
@@ -1755,7 +1761,7 @@
       </c>
       <c r="K19" s="33"/>
     </row>
-    <row r="20" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>14</v>
       </c>
@@ -1788,7 +1794,7 @@
       </c>
       <c r="K20" s="33"/>
     </row>
-    <row r="21" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>15</v>
       </c>
@@ -1821,7 +1827,7 @@
       </c>
       <c r="K21" s="33"/>
     </row>
-    <row r="22" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>16</v>
       </c>
@@ -1854,7 +1860,7 @@
       </c>
       <c r="K22" s="33"/>
     </row>
-    <row r="23" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>17</v>
       </c>
@@ -1887,7 +1893,7 @@
       </c>
       <c r="K23" s="33"/>
     </row>
-    <row r="24" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>24</v>
       </c>
@@ -1920,7 +1926,7 @@
       </c>
       <c r="K24" s="33"/>
     </row>
-    <row r="25" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
         <v>32</v>
       </c>
@@ -1953,7 +1959,7 @@
       </c>
       <c r="K25" s="33"/>
     </row>
-    <row r="26" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
         <v>33</v>
       </c>
@@ -1986,7 +1992,7 @@
       </c>
       <c r="K26" s="33"/>
     </row>
-    <row r="27" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
         <v>34</v>
       </c>
@@ -2019,7 +2025,7 @@
       </c>
       <c r="K27" s="33"/>
     </row>
-    <row r="28" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
         <v>35</v>
       </c>
@@ -2052,7 +2058,7 @@
       </c>
       <c r="K28" s="33"/>
     </row>
-    <row r="29" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
         <v>36</v>
       </c>
@@ -2085,7 +2091,7 @@
       </c>
       <c r="K29" s="33"/>
     </row>
-    <row r="30" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
         <v>37</v>
       </c>
@@ -2118,7 +2124,7 @@
       </c>
       <c r="K30" s="33"/>
     </row>
-    <row r="31" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
         <v>38</v>
       </c>
@@ -2151,7 +2157,7 @@
       </c>
       <c r="K31" s="33"/>
     </row>
-    <row r="32" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
         <v>39</v>
       </c>
@@ -2184,7 +2190,7 @@
       </c>
       <c r="K32" s="33"/>
     </row>
-    <row r="33" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
         <v>40</v>
       </c>
@@ -2217,7 +2223,7 @@
       </c>
       <c r="K33" s="33"/>
     </row>
-    <row r="34" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>41</v>
       </c>
@@ -2250,7 +2256,7 @@
       </c>
       <c r="K34" s="33"/>
     </row>
-    <row r="35" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
         <v>42</v>
       </c>
@@ -2283,7 +2289,7 @@
       </c>
       <c r="K35" s="33"/>
     </row>
-    <row r="36" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
         <v>43</v>
       </c>
@@ -2316,7 +2322,7 @@
       </c>
       <c r="K36" s="33"/>
     </row>
-    <row r="37" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
         <v>44</v>
       </c>
@@ -2349,7 +2355,7 @@
       </c>
       <c r="K37" s="33"/>
     </row>
-    <row r="38" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
         <v>45</v>
       </c>
@@ -2382,7 +2388,7 @@
       </c>
       <c r="K38" s="33"/>
     </row>
-    <row r="39" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
         <v>46</v>
       </c>
@@ -2415,7 +2421,7 @@
       </c>
       <c r="K39" s="33"/>
     </row>
-    <row r="40" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
         <v>47</v>
       </c>
@@ -2448,7 +2454,7 @@
       </c>
       <c r="K40" s="33"/>
     </row>
-    <row r="41" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
         <v>48</v>
       </c>
@@ -2481,7 +2487,7 @@
       </c>
       <c r="K41" s="33"/>
     </row>
-    <row r="42" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
         <v>49</v>
       </c>
@@ -2514,7 +2520,7 @@
       </c>
       <c r="K42" s="33"/>
     </row>
-    <row r="43" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
         <v>50</v>
       </c>
@@ -2547,7 +2553,7 @@
       </c>
       <c r="K43" s="33"/>
     </row>
-    <row r="44" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="9" t="s">
         <v>51</v>
       </c>
@@ -2580,7 +2586,7 @@
       </c>
       <c r="K44" s="33"/>
     </row>
-    <row r="45" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
         <v>52</v>
       </c>
@@ -2613,7 +2619,7 @@
       </c>
       <c r="K45" s="33"/>
     </row>
-    <row r="46" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
         <v>53</v>
       </c>
@@ -2646,7 +2652,7 @@
       </c>
       <c r="K46" s="33"/>
     </row>
-    <row r="47" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
         <v>54</v>
       </c>
@@ -2679,7 +2685,7 @@
       </c>
       <c r="K47" s="33"/>
     </row>
-    <row r="48" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
         <v>55</v>
       </c>
@@ -2712,7 +2718,7 @@
       </c>
       <c r="K48" s="33"/>
     </row>
-    <row r="49" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
         <v>56</v>
       </c>
@@ -2745,7 +2751,7 @@
       </c>
       <c r="K49" s="33"/>
     </row>
-    <row r="50" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="30" t="s">
         <v>57</v>
       </c>
@@ -2778,7 +2784,7 @@
       </c>
       <c r="K50" s="34"/>
     </row>
-    <row r="51" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="31" t="s">
         <v>58</v>
       </c>
@@ -2811,7 +2817,7 @@
       </c>
       <c r="K51" s="35"/>
     </row>
-    <row r="52" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="8" t="s">
         <v>59</v>
       </c>
@@ -2846,7 +2852,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
         <v>60</v>
       </c>
@@ -2881,7 +2887,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="9" t="s">
         <v>61</v>
       </c>
@@ -2916,7 +2922,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="s">
         <v>62</v>
       </c>
@@ -2951,7 +2957,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
         <v>63</v>
       </c>
@@ -2973,12 +2979,20 @@
       <c r="G56" s="2">
         <v>30</v>
       </c>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="20"/>
-      <c r="K56" s="33"/>
-    </row>
-    <row r="57" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H56" s="3">
+        <v>0.82</v>
+      </c>
+      <c r="I56" s="3">
+        <v>0.81</v>
+      </c>
+      <c r="J56" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="K56" s="33" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
         <v>64</v>
       </c>
@@ -3013,7 +3027,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="s">
         <v>92</v>
       </c>
@@ -3040,7 +3054,7 @@
       <c r="J58" s="20"/>
       <c r="K58" s="33"/>
     </row>
-    <row r="59" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
         <v>93</v>
       </c>
@@ -3057,7 +3071,7 @@
       <c r="J59" s="20"/>
       <c r="K59" s="33"/>
     </row>
-    <row r="60" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="9" t="s">
         <v>94</v>
       </c>
@@ -3074,7 +3088,7 @@
       <c r="J60" s="20"/>
       <c r="K60" s="33"/>
     </row>
-    <row r="61" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
         <v>95</v>
       </c>
@@ -3091,7 +3105,7 @@
       <c r="J61" s="20"/>
       <c r="K61" s="33"/>
     </row>
-    <row r="62" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
         <v>96</v>
       </c>
@@ -3108,7 +3122,7 @@
       <c r="J62" s="20"/>
       <c r="K62" s="33"/>
     </row>
-    <row r="63" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
         <v>97</v>
       </c>
@@ -3125,7 +3139,7 @@
       <c r="J63" s="20"/>
       <c r="K63" s="33"/>
     </row>
-    <row r="64" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="9"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -3138,7 +3152,7 @@
       <c r="J64" s="20"/>
       <c r="K64" s="33"/>
     </row>
-    <row r="65" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="9"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -3151,7 +3165,7 @@
       <c r="J65" s="20"/>
       <c r="K65" s="33"/>
     </row>
-    <row r="66" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -3164,7 +3178,7 @@
       <c r="J66" s="20"/>
       <c r="K66" s="33"/>
     </row>
-    <row r="67" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="9"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -3177,7 +3191,7 @@
       <c r="J67" s="20"/>
       <c r="K67" s="33"/>
     </row>
-    <row r="68" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="9"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -3190,7 +3204,7 @@
       <c r="J68" s="20"/>
       <c r="K68" s="33"/>
     </row>
-    <row r="69" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="9"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -3203,7 +3217,7 @@
       <c r="J69" s="20"/>
       <c r="K69" s="33"/>
     </row>
-    <row r="70" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="9"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -3216,7 +3230,7 @@
       <c r="J70" s="20"/>
       <c r="K70" s="33"/>
     </row>
-    <row r="71" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="9"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -3229,7 +3243,7 @@
       <c r="J71" s="20"/>
       <c r="K71" s="33"/>
     </row>
-    <row r="72" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="9"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -3242,7 +3256,7 @@
       <c r="J72" s="20"/>
       <c r="K72" s="33"/>
     </row>
-    <row r="73" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="9"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -3255,7 +3269,7 @@
       <c r="J73" s="20"/>
       <c r="K73" s="33"/>
     </row>
-    <row r="74" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="9"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -3268,7 +3282,7 @@
       <c r="J74" s="20"/>
       <c r="K74" s="33"/>
     </row>
-    <row r="75" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="9"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -3281,7 +3295,7 @@
       <c r="J75" s="20"/>
       <c r="K75" s="33"/>
     </row>
-    <row r="76" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="9"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -3294,7 +3308,7 @@
       <c r="J76" s="20"/>
       <c r="K76" s="33"/>
     </row>
-    <row r="77" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="9"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -3307,7 +3321,7 @@
       <c r="J77" s="20"/>
       <c r="K77" s="33"/>
     </row>
-    <row r="78" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="9"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -3320,7 +3334,7 @@
       <c r="J78" s="20"/>
       <c r="K78" s="33"/>
     </row>
-    <row r="79" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="9"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -3333,7 +3347,7 @@
       <c r="J79" s="20"/>
       <c r="K79" s="33"/>
     </row>
-    <row r="80" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="9"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -3346,7 +3360,7 @@
       <c r="J80" s="20"/>
       <c r="K80" s="33"/>
     </row>
-    <row r="81" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="9"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -3359,7 +3373,7 @@
       <c r="J81" s="20"/>
       <c r="K81" s="33"/>
     </row>
-    <row r="82" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="9"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -3372,7 +3386,7 @@
       <c r="J82" s="20"/>
       <c r="K82" s="33"/>
     </row>
-    <row r="83" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="9"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -3385,7 +3399,7 @@
       <c r="J83" s="20"/>
       <c r="K83" s="33"/>
     </row>
-    <row r="84" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="9"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -3398,7 +3412,7 @@
       <c r="J84" s="20"/>
       <c r="K84" s="33"/>
     </row>
-    <row r="85" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="9"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -3411,7 +3425,7 @@
       <c r="J85" s="20"/>
       <c r="K85" s="33"/>
     </row>
-    <row r="86" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="9"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -3424,7 +3438,7 @@
       <c r="J86" s="20"/>
       <c r="K86" s="33"/>
     </row>
-    <row r="87" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="9"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -3437,7 +3451,7 @@
       <c r="J87" s="20"/>
       <c r="K87" s="33"/>
     </row>
-    <row r="88" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="9"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -3450,7 +3464,7 @@
       <c r="J88" s="20"/>
       <c r="K88" s="33"/>
     </row>
-    <row r="89" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="9"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -3463,7 +3477,7 @@
       <c r="J89" s="20"/>
       <c r="K89" s="33"/>
     </row>
-    <row r="90" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="9"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -3476,7 +3490,7 @@
       <c r="J90" s="20"/>
       <c r="K90" s="33"/>
     </row>
-    <row r="91" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="9"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -3489,7 +3503,7 @@
       <c r="J91" s="20"/>
       <c r="K91" s="33"/>
     </row>
-    <row r="92" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="9"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -3502,7 +3516,7 @@
       <c r="J92" s="20"/>
       <c r="K92" s="33"/>
     </row>
-    <row r="93" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="9"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -3515,7 +3529,7 @@
       <c r="J93" s="20"/>
       <c r="K93" s="33"/>
     </row>
-    <row r="94" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="9"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -3528,7 +3542,7 @@
       <c r="J94" s="20"/>
       <c r="K94" s="33"/>
     </row>
-    <row r="95" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="9"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -3541,7 +3555,7 @@
       <c r="J95" s="20"/>
       <c r="K95" s="33"/>
     </row>
-    <row r="96" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="9"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -3554,7 +3568,7 @@
       <c r="J96" s="20"/>
       <c r="K96" s="33"/>
     </row>
-    <row r="97" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="9"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -3567,7 +3581,7 @@
       <c r="J97" s="20"/>
       <c r="K97" s="33"/>
     </row>
-    <row r="98" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="9"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -3580,7 +3594,7 @@
       <c r="J98" s="20"/>
       <c r="K98" s="33"/>
     </row>
-    <row r="99" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="9"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -3593,7 +3607,7 @@
       <c r="J99" s="20"/>
       <c r="K99" s="33"/>
     </row>
-    <row r="100" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="9"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -3606,7 +3620,7 @@
       <c r="J100" s="20"/>
       <c r="K100" s="33"/>
     </row>
-    <row r="101" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="9"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -3619,7 +3633,7 @@
       <c r="J101" s="20"/>
       <c r="K101" s="33"/>
     </row>
-    <row r="102" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="9"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -3632,7 +3646,7 @@
       <c r="J102" s="20"/>
       <c r="K102" s="33"/>
     </row>
-    <row r="103" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="9"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -3645,7 +3659,7 @@
       <c r="J103" s="20"/>
       <c r="K103" s="33"/>
     </row>
-    <row r="104" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="9"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -3658,7 +3672,7 @@
       <c r="J104" s="20"/>
       <c r="K104" s="33"/>
     </row>
-    <row r="105" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="9"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -3671,7 +3685,7 @@
       <c r="J105" s="20"/>
       <c r="K105" s="33"/>
     </row>
-    <row r="106" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="9"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -3684,7 +3698,7 @@
       <c r="J106" s="20"/>
       <c r="K106" s="33"/>
     </row>
-    <row r="107" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="9"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -3697,7 +3711,7 @@
       <c r="J107" s="20"/>
       <c r="K107" s="33"/>
     </row>
-    <row r="108" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="9"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -3710,7 +3724,7 @@
       <c r="J108" s="20"/>
       <c r="K108" s="33"/>
     </row>
-    <row r="109" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="9"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -3723,7 +3737,7 @@
       <c r="J109" s="20"/>
       <c r="K109" s="33"/>
     </row>
-    <row r="110" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="9"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -3736,7 +3750,7 @@
       <c r="J110" s="20"/>
       <c r="K110" s="33"/>
     </row>
-    <row r="111" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="9"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -3749,7 +3763,7 @@
       <c r="J111" s="20"/>
       <c r="K111" s="33"/>
     </row>
-    <row r="112" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="9"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -3762,7 +3776,7 @@
       <c r="J112" s="20"/>
       <c r="K112" s="33"/>
     </row>
-    <row r="113" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="9"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -3775,7 +3789,7 @@
       <c r="J113" s="20"/>
       <c r="K113" s="33"/>
     </row>
-    <row r="114" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="9"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -3788,7 +3802,7 @@
       <c r="J114" s="20"/>
       <c r="K114" s="33"/>
     </row>
-    <row r="115" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="9"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -3801,7 +3815,7 @@
       <c r="J115" s="20"/>
       <c r="K115" s="33"/>
     </row>
-    <row r="116" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="9"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -3814,7 +3828,7 @@
       <c r="J116" s="20"/>
       <c r="K116" s="33"/>
     </row>
-    <row r="117" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="9"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -3827,7 +3841,7 @@
       <c r="J117" s="20"/>
       <c r="K117" s="33"/>
     </row>
-    <row r="118" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="9"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -3840,7 +3854,7 @@
       <c r="J118" s="20"/>
       <c r="K118" s="33"/>
     </row>
-    <row r="119" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="9"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -3853,7 +3867,7 @@
       <c r="J119" s="20"/>
       <c r="K119" s="33"/>
     </row>
-    <row r="120" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="9"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -3866,7 +3880,7 @@
       <c r="J120" s="20"/>
       <c r="K120" s="33"/>
     </row>
-    <row r="121" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="9"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -3879,7 +3893,7 @@
       <c r="J121" s="20"/>
       <c r="K121" s="33"/>
     </row>
-    <row r="122" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="9"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -3892,7 +3906,7 @@
       <c r="J122" s="20"/>
       <c r="K122" s="33"/>
     </row>
-    <row r="123" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="9"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -3905,7 +3919,7 @@
       <c r="J123" s="20"/>
       <c r="K123" s="33"/>
     </row>
-    <row r="124" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="9"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -3918,7 +3932,7 @@
       <c r="J124" s="20"/>
       <c r="K124" s="33"/>
     </row>
-    <row r="125" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="9"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -3931,7 +3945,7 @@
       <c r="J125" s="20"/>
       <c r="K125" s="33"/>
     </row>
-    <row r="126" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="9"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -3944,7 +3958,7 @@
       <c r="J126" s="20"/>
       <c r="K126" s="33"/>
     </row>
-    <row r="127" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="9"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -3957,7 +3971,7 @@
       <c r="J127" s="20"/>
       <c r="K127" s="33"/>
     </row>
-    <row r="128" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="9"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -3970,7 +3984,7 @@
       <c r="J128" s="20"/>
       <c r="K128" s="33"/>
     </row>
-    <row r="129" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="9"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -3983,7 +3997,7 @@
       <c r="J129" s="20"/>
       <c r="K129" s="33"/>
     </row>
-    <row r="130" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="9"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -3996,7 +4010,7 @@
       <c r="J130" s="20"/>
       <c r="K130" s="33"/>
     </row>
-    <row r="131" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="9"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -4009,7 +4023,7 @@
       <c r="J131" s="20"/>
       <c r="K131" s="33"/>
     </row>
-    <row r="132" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="9"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -4022,7 +4036,7 @@
       <c r="J132" s="20"/>
       <c r="K132" s="33"/>
     </row>
-    <row r="133" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="9"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -4035,7 +4049,7 @@
       <c r="J133" s="20"/>
       <c r="K133" s="33"/>
     </row>
-    <row r="134" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" s="9"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -4048,7 +4062,7 @@
       <c r="J134" s="20"/>
       <c r="K134" s="33"/>
     </row>
-    <row r="135" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" s="9"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -4061,7 +4075,7 @@
       <c r="J135" s="20"/>
       <c r="K135" s="33"/>
     </row>
-    <row r="136" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" s="9"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -4074,7 +4088,7 @@
       <c r="J136" s="20"/>
       <c r="K136" s="33"/>
     </row>
-    <row r="137" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="9"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -4087,7 +4101,7 @@
       <c r="J137" s="20"/>
       <c r="K137" s="33"/>
     </row>
-    <row r="138" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="9"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -4100,7 +4114,7 @@
       <c r="J138" s="20"/>
       <c r="K138" s="33"/>
     </row>
-    <row r="139" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="9"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -4113,7 +4127,7 @@
       <c r="J139" s="20"/>
       <c r="K139" s="33"/>
     </row>
-    <row r="140" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A140" s="10"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
@@ -4126,28 +4140,28 @@
       <c r="J140" s="21"/>
       <c r="K140" s="36"/>
     </row>
-    <row r="141" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="142" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="143" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="144" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="145" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="146" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="147" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="148" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="149" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="150" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="151" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="152" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="153" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="154" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="155" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="156" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="157" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="158" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="160" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="161" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="162" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="142" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="143" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="144" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="145" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="146" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="147" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="148" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="149" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="150" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="151" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="152" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="153" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="154" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="155" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="156" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="157" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="158" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="159" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="160" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="161" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="162" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Segmentation Test Report.xlsx
</commit_message>
<xml_diff>
--- a/doc/Segmentation Test Report.xlsx
+++ b/doc/Segmentation Test Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovannirapa/Documents/GitHub/speech_privacy_android_accelerometer/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39392\Documents\GitHub\speech_privacy_android_accelerometer\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE13741-3223-2249-AFA4-99628F81D22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFCAC96-0725-40B2-A741-4447F4058EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{449DE670-0F7F-4D85-9FF1-3C3B2473E6CE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{449DE670-0F7F-4D85-9FF1-3C3B2473E6CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="113">
   <si>
     <t>Test N°</t>
   </si>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t>9</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
 </sst>
 </file>
@@ -1141,23 +1144,23 @@
   <dimension ref="A1:K162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" zoomScale="107" workbookViewId="0">
-      <selection activeCell="K58" sqref="K58"/>
+      <selection activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="19" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="37"/>
+    <col min="1" max="3" width="16.36328125" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" customWidth="1"/>
+    <col min="6" max="6" width="10.36328125" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" customWidth="1"/>
+    <col min="8" max="8" width="11.36328125" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" customWidth="1"/>
+    <col min="10" max="10" width="11.6328125" style="19" customWidth="1"/>
+    <col min="11" max="11" width="8.6328125" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1192,7 +1195,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>8</v>
       </c>
@@ -1223,7 +1226,7 @@
       <c r="J2" s="22"/>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>9</v>
       </c>
@@ -1254,7 +1257,7 @@
       <c r="J3" s="20"/>
       <c r="K3" s="33"/>
     </row>
-    <row r="4" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>10</v>
       </c>
@@ -1285,7 +1288,7 @@
       <c r="J4" s="20"/>
       <c r="K4" s="33"/>
     </row>
-    <row r="5" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
         <v>11</v>
       </c>
@@ -1316,7 +1319,7 @@
       <c r="J5" s="20"/>
       <c r="K5" s="33"/>
     </row>
-    <row r="6" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
         <v>12</v>
       </c>
@@ -1347,7 +1350,7 @@
       <c r="J6" s="20"/>
       <c r="K6" s="33"/>
     </row>
-    <row r="7" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
@@ -1378,7 +1381,7 @@
       <c r="J7" s="20"/>
       <c r="K7" s="33"/>
     </row>
-    <row r="8" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
@@ -1409,7 +1412,7 @@
       <c r="J8" s="20"/>
       <c r="K8" s="33"/>
     </row>
-    <row r="9" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
@@ -1440,7 +1443,7 @@
       <c r="J9" s="20"/>
       <c r="K9" s="33"/>
     </row>
-    <row r="10" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
         <v>16</v>
       </c>
@@ -1471,7 +1474,7 @@
       <c r="J10" s="20"/>
       <c r="K10" s="33"/>
     </row>
-    <row r="11" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
         <v>17</v>
       </c>
@@ -1502,7 +1505,7 @@
       <c r="J11" s="20"/>
       <c r="K11" s="33"/>
     </row>
-    <row r="12" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="16" t="s">
         <v>24</v>
       </c>
@@ -1533,7 +1536,7 @@
       <c r="J12" s="25"/>
       <c r="K12" s="34"/>
     </row>
-    <row r="13" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="26" t="s">
         <v>26</v>
       </c>
@@ -1566,7 +1569,7 @@
       </c>
       <c r="K13" s="35"/>
     </row>
-    <row r="14" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>8</v>
       </c>
@@ -1599,7 +1602,7 @@
       </c>
       <c r="K14" s="32"/>
     </row>
-    <row r="15" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>9</v>
       </c>
@@ -1632,7 +1635,7 @@
       </c>
       <c r="K15" s="33"/>
     </row>
-    <row r="16" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>10</v>
       </c>
@@ -1665,7 +1668,7 @@
       </c>
       <c r="K16" s="33"/>
     </row>
-    <row r="17" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>11</v>
       </c>
@@ -1698,7 +1701,7 @@
       </c>
       <c r="K17" s="33"/>
     </row>
-    <row r="18" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
         <v>12</v>
       </c>
@@ -1731,7 +1734,7 @@
       </c>
       <c r="K18" s="33"/>
     </row>
-    <row r="19" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>13</v>
       </c>
@@ -1764,7 +1767,7 @@
       </c>
       <c r="K19" s="33"/>
     </row>
-    <row r="20" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>14</v>
       </c>
@@ -1797,7 +1800,7 @@
       </c>
       <c r="K20" s="33"/>
     </row>
-    <row r="21" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>15</v>
       </c>
@@ -1830,7 +1833,7 @@
       </c>
       <c r="K21" s="33"/>
     </row>
-    <row r="22" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>16</v>
       </c>
@@ -1863,7 +1866,7 @@
       </c>
       <c r="K22" s="33"/>
     </row>
-    <row r="23" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>17</v>
       </c>
@@ -1896,7 +1899,7 @@
       </c>
       <c r="K23" s="33"/>
     </row>
-    <row r="24" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>24</v>
       </c>
@@ -1929,7 +1932,7 @@
       </c>
       <c r="K24" s="33"/>
     </row>
-    <row r="25" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
         <v>32</v>
       </c>
@@ -1962,7 +1965,7 @@
       </c>
       <c r="K25" s="33"/>
     </row>
-    <row r="26" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
         <v>33</v>
       </c>
@@ -1995,7 +1998,7 @@
       </c>
       <c r="K26" s="33"/>
     </row>
-    <row r="27" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
         <v>34</v>
       </c>
@@ -2028,7 +2031,7 @@
       </c>
       <c r="K27" s="33"/>
     </row>
-    <row r="28" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
         <v>35</v>
       </c>
@@ -2061,7 +2064,7 @@
       </c>
       <c r="K28" s="33"/>
     </row>
-    <row r="29" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
         <v>36</v>
       </c>
@@ -2094,7 +2097,7 @@
       </c>
       <c r="K29" s="33"/>
     </row>
-    <row r="30" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
         <v>37</v>
       </c>
@@ -2127,7 +2130,7 @@
       </c>
       <c r="K30" s="33"/>
     </row>
-    <row r="31" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
         <v>38</v>
       </c>
@@ -2160,7 +2163,7 @@
       </c>
       <c r="K31" s="33"/>
     </row>
-    <row r="32" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
         <v>39</v>
       </c>
@@ -2193,7 +2196,7 @@
       </c>
       <c r="K32" s="33"/>
     </row>
-    <row r="33" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
         <v>40</v>
       </c>
@@ -2226,7 +2229,7 @@
       </c>
       <c r="K33" s="33"/>
     </row>
-    <row r="34" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>41</v>
       </c>
@@ -2259,7 +2262,7 @@
       </c>
       <c r="K34" s="33"/>
     </row>
-    <row r="35" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
         <v>42</v>
       </c>
@@ -2292,7 +2295,7 @@
       </c>
       <c r="K35" s="33"/>
     </row>
-    <row r="36" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
         <v>43</v>
       </c>
@@ -2325,7 +2328,7 @@
       </c>
       <c r="K36" s="33"/>
     </row>
-    <row r="37" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
         <v>44</v>
       </c>
@@ -2358,7 +2361,7 @@
       </c>
       <c r="K37" s="33"/>
     </row>
-    <row r="38" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
         <v>45</v>
       </c>
@@ -2391,7 +2394,7 @@
       </c>
       <c r="K38" s="33"/>
     </row>
-    <row r="39" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
         <v>46</v>
       </c>
@@ -2424,7 +2427,7 @@
       </c>
       <c r="K39" s="33"/>
     </row>
-    <row r="40" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
         <v>47</v>
       </c>
@@ -2457,7 +2460,7 @@
       </c>
       <c r="K40" s="33"/>
     </row>
-    <row r="41" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
         <v>48</v>
       </c>
@@ -2490,7 +2493,7 @@
       </c>
       <c r="K41" s="33"/>
     </row>
-    <row r="42" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
         <v>49</v>
       </c>
@@ -2523,7 +2526,7 @@
       </c>
       <c r="K42" s="33"/>
     </row>
-    <row r="43" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
         <v>50</v>
       </c>
@@ -2556,7 +2559,7 @@
       </c>
       <c r="K43" s="33"/>
     </row>
-    <row r="44" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="9" t="s">
         <v>51</v>
       </c>
@@ -2589,7 +2592,7 @@
       </c>
       <c r="K44" s="33"/>
     </row>
-    <row r="45" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
         <v>52</v>
       </c>
@@ -2622,7 +2625,7 @@
       </c>
       <c r="K45" s="33"/>
     </row>
-    <row r="46" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
         <v>53</v>
       </c>
@@ -2655,7 +2658,7 @@
       </c>
       <c r="K46" s="33"/>
     </row>
-    <row r="47" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
         <v>54</v>
       </c>
@@ -2688,7 +2691,7 @@
       </c>
       <c r="K47" s="33"/>
     </row>
-    <row r="48" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
         <v>55</v>
       </c>
@@ -2721,7 +2724,7 @@
       </c>
       <c r="K48" s="33"/>
     </row>
-    <row r="49" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
         <v>56</v>
       </c>
@@ -2754,7 +2757,7 @@
       </c>
       <c r="K49" s="33"/>
     </row>
-    <row r="50" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="30" t="s">
         <v>57</v>
       </c>
@@ -2787,7 +2790,7 @@
       </c>
       <c r="K50" s="34"/>
     </row>
-    <row r="51" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="31" t="s">
         <v>58</v>
       </c>
@@ -2820,7 +2823,7 @@
       </c>
       <c r="K51" s="35"/>
     </row>
-    <row r="52" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="8" t="s">
         <v>59</v>
       </c>
@@ -2855,7 +2858,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
         <v>60</v>
       </c>
@@ -2890,7 +2893,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="9" t="s">
         <v>61</v>
       </c>
@@ -2925,7 +2928,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="s">
         <v>62</v>
       </c>
@@ -2960,7 +2963,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
         <v>63</v>
       </c>
@@ -2995,7 +2998,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
         <v>64</v>
       </c>
@@ -3030,7 +3033,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="s">
         <v>92</v>
       </c>
@@ -3065,24 +3068,42 @@
         <v>108</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
+      <c r="B59" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="D59" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
-      <c r="H59" s="3"/>
-      <c r="I59" s="3"/>
-      <c r="J59" s="20"/>
-      <c r="K59" s="33"/>
-    </row>
-    <row r="60" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E59" s="2">
+        <v>500</v>
+      </c>
+      <c r="F59" s="2">
+        <v>100</v>
+      </c>
+      <c r="G59" s="2">
+        <v>30</v>
+      </c>
+      <c r="H59" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="I59" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="J59" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="K59" s="33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="9" t="s">
         <v>94</v>
       </c>
@@ -3099,7 +3120,7 @@
       <c r="J60" s="20"/>
       <c r="K60" s="33"/>
     </row>
-    <row r="61" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
         <v>95</v>
       </c>
@@ -3116,7 +3137,7 @@
       <c r="J61" s="20"/>
       <c r="K61" s="33"/>
     </row>
-    <row r="62" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
         <v>96</v>
       </c>
@@ -3133,7 +3154,7 @@
       <c r="J62" s="20"/>
       <c r="K62" s="33"/>
     </row>
-    <row r="63" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
         <v>97</v>
       </c>
@@ -3150,7 +3171,7 @@
       <c r="J63" s="20"/>
       <c r="K63" s="33"/>
     </row>
-    <row r="64" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="9"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -3163,7 +3184,7 @@
       <c r="J64" s="20"/>
       <c r="K64" s="33"/>
     </row>
-    <row r="65" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="9"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -3176,7 +3197,7 @@
       <c r="J65" s="20"/>
       <c r="K65" s="33"/>
     </row>
-    <row r="66" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -3189,7 +3210,7 @@
       <c r="J66" s="20"/>
       <c r="K66" s="33"/>
     </row>
-    <row r="67" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="9"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -3202,7 +3223,7 @@
       <c r="J67" s="20"/>
       <c r="K67" s="33"/>
     </row>
-    <row r="68" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="9"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -3215,7 +3236,7 @@
       <c r="J68" s="20"/>
       <c r="K68" s="33"/>
     </row>
-    <row r="69" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="9"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -3228,7 +3249,7 @@
       <c r="J69" s="20"/>
       <c r="K69" s="33"/>
     </row>
-    <row r="70" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="9"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -3241,7 +3262,7 @@
       <c r="J70" s="20"/>
       <c r="K70" s="33"/>
     </row>
-    <row r="71" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="9"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -3254,7 +3275,7 @@
       <c r="J71" s="20"/>
       <c r="K71" s="33"/>
     </row>
-    <row r="72" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="9"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -3267,7 +3288,7 @@
       <c r="J72" s="20"/>
       <c r="K72" s="33"/>
     </row>
-    <row r="73" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="9"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -3280,7 +3301,7 @@
       <c r="J73" s="20"/>
       <c r="K73" s="33"/>
     </row>
-    <row r="74" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="9"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -3293,7 +3314,7 @@
       <c r="J74" s="20"/>
       <c r="K74" s="33"/>
     </row>
-    <row r="75" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="9"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -3306,7 +3327,7 @@
       <c r="J75" s="20"/>
       <c r="K75" s="33"/>
     </row>
-    <row r="76" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="9"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -3319,7 +3340,7 @@
       <c r="J76" s="20"/>
       <c r="K76" s="33"/>
     </row>
-    <row r="77" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="9"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -3332,7 +3353,7 @@
       <c r="J77" s="20"/>
       <c r="K77" s="33"/>
     </row>
-    <row r="78" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="9"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -3345,7 +3366,7 @@
       <c r="J78" s="20"/>
       <c r="K78" s="33"/>
     </row>
-    <row r="79" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="9"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -3358,7 +3379,7 @@
       <c r="J79" s="20"/>
       <c r="K79" s="33"/>
     </row>
-    <row r="80" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="9"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -3371,7 +3392,7 @@
       <c r="J80" s="20"/>
       <c r="K80" s="33"/>
     </row>
-    <row r="81" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="9"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -3384,7 +3405,7 @@
       <c r="J81" s="20"/>
       <c r="K81" s="33"/>
     </row>
-    <row r="82" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="9"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -3397,7 +3418,7 @@
       <c r="J82" s="20"/>
       <c r="K82" s="33"/>
     </row>
-    <row r="83" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="9"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -3410,7 +3431,7 @@
       <c r="J83" s="20"/>
       <c r="K83" s="33"/>
     </row>
-    <row r="84" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="9"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -3423,7 +3444,7 @@
       <c r="J84" s="20"/>
       <c r="K84" s="33"/>
     </row>
-    <row r="85" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="9"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -3436,7 +3457,7 @@
       <c r="J85" s="20"/>
       <c r="K85" s="33"/>
     </row>
-    <row r="86" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="9"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -3449,7 +3470,7 @@
       <c r="J86" s="20"/>
       <c r="K86" s="33"/>
     </row>
-    <row r="87" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="9"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -3462,7 +3483,7 @@
       <c r="J87" s="20"/>
       <c r="K87" s="33"/>
     </row>
-    <row r="88" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="9"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -3475,7 +3496,7 @@
       <c r="J88" s="20"/>
       <c r="K88" s="33"/>
     </row>
-    <row r="89" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="9"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -3488,7 +3509,7 @@
       <c r="J89" s="20"/>
       <c r="K89" s="33"/>
     </row>
-    <row r="90" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="9"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -3501,7 +3522,7 @@
       <c r="J90" s="20"/>
       <c r="K90" s="33"/>
     </row>
-    <row r="91" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="9"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -3514,7 +3535,7 @@
       <c r="J91" s="20"/>
       <c r="K91" s="33"/>
     </row>
-    <row r="92" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="9"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -3527,7 +3548,7 @@
       <c r="J92" s="20"/>
       <c r="K92" s="33"/>
     </row>
-    <row r="93" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="9"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -3540,7 +3561,7 @@
       <c r="J93" s="20"/>
       <c r="K93" s="33"/>
     </row>
-    <row r="94" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="9"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -3553,7 +3574,7 @@
       <c r="J94" s="20"/>
       <c r="K94" s="33"/>
     </row>
-    <row r="95" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="9"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -3566,7 +3587,7 @@
       <c r="J95" s="20"/>
       <c r="K95" s="33"/>
     </row>
-    <row r="96" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="9"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -3579,7 +3600,7 @@
       <c r="J96" s="20"/>
       <c r="K96" s="33"/>
     </row>
-    <row r="97" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="9"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -3592,7 +3613,7 @@
       <c r="J97" s="20"/>
       <c r="K97" s="33"/>
     </row>
-    <row r="98" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="9"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -3605,7 +3626,7 @@
       <c r="J98" s="20"/>
       <c r="K98" s="33"/>
     </row>
-    <row r="99" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="9"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -3618,7 +3639,7 @@
       <c r="J99" s="20"/>
       <c r="K99" s="33"/>
     </row>
-    <row r="100" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="9"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -3631,7 +3652,7 @@
       <c r="J100" s="20"/>
       <c r="K100" s="33"/>
     </row>
-    <row r="101" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="9"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -3644,7 +3665,7 @@
       <c r="J101" s="20"/>
       <c r="K101" s="33"/>
     </row>
-    <row r="102" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="9"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -3657,7 +3678,7 @@
       <c r="J102" s="20"/>
       <c r="K102" s="33"/>
     </row>
-    <row r="103" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="9"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -3670,7 +3691,7 @@
       <c r="J103" s="20"/>
       <c r="K103" s="33"/>
     </row>
-    <row r="104" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="9"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -3683,7 +3704,7 @@
       <c r="J104" s="20"/>
       <c r="K104" s="33"/>
     </row>
-    <row r="105" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="9"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -3696,7 +3717,7 @@
       <c r="J105" s="20"/>
       <c r="K105" s="33"/>
     </row>
-    <row r="106" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="9"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -3709,7 +3730,7 @@
       <c r="J106" s="20"/>
       <c r="K106" s="33"/>
     </row>
-    <row r="107" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="9"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -3722,7 +3743,7 @@
       <c r="J107" s="20"/>
       <c r="K107" s="33"/>
     </row>
-    <row r="108" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="9"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -3735,7 +3756,7 @@
       <c r="J108" s="20"/>
       <c r="K108" s="33"/>
     </row>
-    <row r="109" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="9"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -3748,7 +3769,7 @@
       <c r="J109" s="20"/>
       <c r="K109" s="33"/>
     </row>
-    <row r="110" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="9"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -3761,7 +3782,7 @@
       <c r="J110" s="20"/>
       <c r="K110" s="33"/>
     </row>
-    <row r="111" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="9"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -3774,7 +3795,7 @@
       <c r="J111" s="20"/>
       <c r="K111" s="33"/>
     </row>
-    <row r="112" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="9"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -3787,7 +3808,7 @@
       <c r="J112" s="20"/>
       <c r="K112" s="33"/>
     </row>
-    <row r="113" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="9"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -3800,7 +3821,7 @@
       <c r="J113" s="20"/>
       <c r="K113" s="33"/>
     </row>
-    <row r="114" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="9"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -3813,7 +3834,7 @@
       <c r="J114" s="20"/>
       <c r="K114" s="33"/>
     </row>
-    <row r="115" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="9"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -3826,7 +3847,7 @@
       <c r="J115" s="20"/>
       <c r="K115" s="33"/>
     </row>
-    <row r="116" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="9"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -3839,7 +3860,7 @@
       <c r="J116" s="20"/>
       <c r="K116" s="33"/>
     </row>
-    <row r="117" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="9"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -3852,7 +3873,7 @@
       <c r="J117" s="20"/>
       <c r="K117" s="33"/>
     </row>
-    <row r="118" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="9"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -3865,7 +3886,7 @@
       <c r="J118" s="20"/>
       <c r="K118" s="33"/>
     </row>
-    <row r="119" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="9"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -3878,7 +3899,7 @@
       <c r="J119" s="20"/>
       <c r="K119" s="33"/>
     </row>
-    <row r="120" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="9"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -3891,7 +3912,7 @@
       <c r="J120" s="20"/>
       <c r="K120" s="33"/>
     </row>
-    <row r="121" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="9"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -3904,7 +3925,7 @@
       <c r="J121" s="20"/>
       <c r="K121" s="33"/>
     </row>
-    <row r="122" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="9"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -3917,7 +3938,7 @@
       <c r="J122" s="20"/>
       <c r="K122" s="33"/>
     </row>
-    <row r="123" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="9"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -3930,7 +3951,7 @@
       <c r="J123" s="20"/>
       <c r="K123" s="33"/>
     </row>
-    <row r="124" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="9"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -3943,7 +3964,7 @@
       <c r="J124" s="20"/>
       <c r="K124" s="33"/>
     </row>
-    <row r="125" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="9"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -3956,7 +3977,7 @@
       <c r="J125" s="20"/>
       <c r="K125" s="33"/>
     </row>
-    <row r="126" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="9"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -3969,7 +3990,7 @@
       <c r="J126" s="20"/>
       <c r="K126" s="33"/>
     </row>
-    <row r="127" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="9"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -3982,7 +4003,7 @@
       <c r="J127" s="20"/>
       <c r="K127" s="33"/>
     </row>
-    <row r="128" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="9"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -3995,7 +4016,7 @@
       <c r="J128" s="20"/>
       <c r="K128" s="33"/>
     </row>
-    <row r="129" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="9"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -4008,7 +4029,7 @@
       <c r="J129" s="20"/>
       <c r="K129" s="33"/>
     </row>
-    <row r="130" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="9"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -4021,7 +4042,7 @@
       <c r="J130" s="20"/>
       <c r="K130" s="33"/>
     </row>
-    <row r="131" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="9"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -4034,7 +4055,7 @@
       <c r="J131" s="20"/>
       <c r="K131" s="33"/>
     </row>
-    <row r="132" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="9"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -4047,7 +4068,7 @@
       <c r="J132" s="20"/>
       <c r="K132" s="33"/>
     </row>
-    <row r="133" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="9"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -4060,7 +4081,7 @@
       <c r="J133" s="20"/>
       <c r="K133" s="33"/>
     </row>
-    <row r="134" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" s="9"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -4073,7 +4094,7 @@
       <c r="J134" s="20"/>
       <c r="K134" s="33"/>
     </row>
-    <row r="135" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" s="9"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -4086,7 +4107,7 @@
       <c r="J135" s="20"/>
       <c r="K135" s="33"/>
     </row>
-    <row r="136" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" s="9"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -4099,7 +4120,7 @@
       <c r="J136" s="20"/>
       <c r="K136" s="33"/>
     </row>
-    <row r="137" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="9"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -4112,7 +4133,7 @@
       <c r="J137" s="20"/>
       <c r="K137" s="33"/>
     </row>
-    <row r="138" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="9"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -4125,7 +4146,7 @@
       <c r="J138" s="20"/>
       <c r="K138" s="33"/>
     </row>
-    <row r="139" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="9"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -4138,7 +4159,7 @@
       <c r="J139" s="20"/>
       <c r="K139" s="33"/>
     </row>
-    <row r="140" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A140" s="10"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
@@ -4151,28 +4172,28 @@
       <c r="J140" s="21"/>
       <c r="K140" s="36"/>
     </row>
-    <row r="141" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="142" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="143" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="144" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="145" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="146" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="147" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="148" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="149" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="150" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="151" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="152" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="153" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="154" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="155" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="156" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="157" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="158" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="160" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="161" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="162" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="142" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="143" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="144" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="145" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="146" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="147" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="148" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="149" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="150" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="151" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="152" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="153" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="154" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="155" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="156" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="157" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="158" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="159" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="160" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="161" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="162" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
upload test image and test result
</commit_message>
<xml_diff>
--- a/doc/Segmentation Test Report.xlsx
+++ b/doc/Segmentation Test Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovannirapa/Documents/GitHub/speech_privacy_android_accelerometer/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39392\Documents\GitHub\speech_privacy_android_accelerometer\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C6A537-5B48-2244-BA9E-D7536E1708FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62FBFC0-ED67-4BFA-99CB-238D94B9DD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{449DE670-0F7F-4D85-9FF1-3C3B2473E6CE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{449DE670-0F7F-4D85-9FF1-3C3B2473E6CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="115">
   <si>
     <t>Test N°</t>
   </si>
@@ -376,6 +376,9 @@
   </si>
   <si>
     <t>15gg</t>
+  </si>
+  <si>
+    <t>14</t>
   </si>
 </sst>
 </file>
@@ -1147,23 +1150,23 @@
   <dimension ref="A1:K162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" zoomScale="107" workbookViewId="0">
-      <selection activeCell="K60" sqref="K60"/>
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="19" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="37"/>
+    <col min="1" max="3" width="16.36328125" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" customWidth="1"/>
+    <col min="6" max="6" width="10.36328125" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" customWidth="1"/>
+    <col min="8" max="8" width="11.36328125" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" customWidth="1"/>
+    <col min="10" max="10" width="11.6328125" style="19" customWidth="1"/>
+    <col min="11" max="11" width="8.6328125" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1198,7 +1201,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>8</v>
       </c>
@@ -1229,7 +1232,7 @@
       <c r="J2" s="22"/>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>9</v>
       </c>
@@ -1260,7 +1263,7 @@
       <c r="J3" s="20"/>
       <c r="K3" s="33"/>
     </row>
-    <row r="4" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>10</v>
       </c>
@@ -1291,7 +1294,7 @@
       <c r="J4" s="20"/>
       <c r="K4" s="33"/>
     </row>
-    <row r="5" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
         <v>11</v>
       </c>
@@ -1322,7 +1325,7 @@
       <c r="J5" s="20"/>
       <c r="K5" s="33"/>
     </row>
-    <row r="6" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
         <v>12</v>
       </c>
@@ -1353,7 +1356,7 @@
       <c r="J6" s="20"/>
       <c r="K6" s="33"/>
     </row>
-    <row r="7" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
@@ -1384,7 +1387,7 @@
       <c r="J7" s="20"/>
       <c r="K7" s="33"/>
     </row>
-    <row r="8" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
@@ -1415,7 +1418,7 @@
       <c r="J8" s="20"/>
       <c r="K8" s="33"/>
     </row>
-    <row r="9" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
@@ -1446,7 +1449,7 @@
       <c r="J9" s="20"/>
       <c r="K9" s="33"/>
     </row>
-    <row r="10" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
         <v>16</v>
       </c>
@@ -1477,7 +1480,7 @@
       <c r="J10" s="20"/>
       <c r="K10" s="33"/>
     </row>
-    <row r="11" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
         <v>17</v>
       </c>
@@ -1508,7 +1511,7 @@
       <c r="J11" s="20"/>
       <c r="K11" s="33"/>
     </row>
-    <row r="12" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="16" t="s">
         <v>24</v>
       </c>
@@ -1539,7 +1542,7 @@
       <c r="J12" s="25"/>
       <c r="K12" s="34"/>
     </row>
-    <row r="13" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="26" t="s">
         <v>26</v>
       </c>
@@ -1572,7 +1575,7 @@
       </c>
       <c r="K13" s="35"/>
     </row>
-    <row r="14" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>8</v>
       </c>
@@ -1605,7 +1608,7 @@
       </c>
       <c r="K14" s="32"/>
     </row>
-    <row r="15" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>9</v>
       </c>
@@ -1638,7 +1641,7 @@
       </c>
       <c r="K15" s="33"/>
     </row>
-    <row r="16" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>10</v>
       </c>
@@ -1671,7 +1674,7 @@
       </c>
       <c r="K16" s="33"/>
     </row>
-    <row r="17" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>11</v>
       </c>
@@ -1704,7 +1707,7 @@
       </c>
       <c r="K17" s="33"/>
     </row>
-    <row r="18" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
         <v>12</v>
       </c>
@@ -1737,7 +1740,7 @@
       </c>
       <c r="K18" s="33"/>
     </row>
-    <row r="19" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>13</v>
       </c>
@@ -1770,7 +1773,7 @@
       </c>
       <c r="K19" s="33"/>
     </row>
-    <row r="20" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>14</v>
       </c>
@@ -1803,7 +1806,7 @@
       </c>
       <c r="K20" s="33"/>
     </row>
-    <row r="21" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>15</v>
       </c>
@@ -1836,7 +1839,7 @@
       </c>
       <c r="K21" s="33"/>
     </row>
-    <row r="22" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>16</v>
       </c>
@@ -1869,7 +1872,7 @@
       </c>
       <c r="K22" s="33"/>
     </row>
-    <row r="23" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>17</v>
       </c>
@@ -1902,7 +1905,7 @@
       </c>
       <c r="K23" s="33"/>
     </row>
-    <row r="24" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>24</v>
       </c>
@@ -1935,7 +1938,7 @@
       </c>
       <c r="K24" s="33"/>
     </row>
-    <row r="25" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
         <v>32</v>
       </c>
@@ -1968,7 +1971,7 @@
       </c>
       <c r="K25" s="33"/>
     </row>
-    <row r="26" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
         <v>33</v>
       </c>
@@ -2001,7 +2004,7 @@
       </c>
       <c r="K26" s="33"/>
     </row>
-    <row r="27" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
         <v>34</v>
       </c>
@@ -2034,7 +2037,7 @@
       </c>
       <c r="K27" s="33"/>
     </row>
-    <row r="28" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
         <v>35</v>
       </c>
@@ -2067,7 +2070,7 @@
       </c>
       <c r="K28" s="33"/>
     </row>
-    <row r="29" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
         <v>36</v>
       </c>
@@ -2100,7 +2103,7 @@
       </c>
       <c r="K29" s="33"/>
     </row>
-    <row r="30" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
         <v>37</v>
       </c>
@@ -2133,7 +2136,7 @@
       </c>
       <c r="K30" s="33"/>
     </row>
-    <row r="31" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
         <v>38</v>
       </c>
@@ -2166,7 +2169,7 @@
       </c>
       <c r="K31" s="33"/>
     </row>
-    <row r="32" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
         <v>39</v>
       </c>
@@ -2199,7 +2202,7 @@
       </c>
       <c r="K32" s="33"/>
     </row>
-    <row r="33" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
         <v>40</v>
       </c>
@@ -2232,7 +2235,7 @@
       </c>
       <c r="K33" s="33"/>
     </row>
-    <row r="34" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>41</v>
       </c>
@@ -2265,7 +2268,7 @@
       </c>
       <c r="K34" s="33"/>
     </row>
-    <row r="35" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
         <v>42</v>
       </c>
@@ -2298,7 +2301,7 @@
       </c>
       <c r="K35" s="33"/>
     </row>
-    <row r="36" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
         <v>43</v>
       </c>
@@ -2331,7 +2334,7 @@
       </c>
       <c r="K36" s="33"/>
     </row>
-    <row r="37" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
         <v>44</v>
       </c>
@@ -2364,7 +2367,7 @@
       </c>
       <c r="K37" s="33"/>
     </row>
-    <row r="38" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
         <v>45</v>
       </c>
@@ -2397,7 +2400,7 @@
       </c>
       <c r="K38" s="33"/>
     </row>
-    <row r="39" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
         <v>46</v>
       </c>
@@ -2430,7 +2433,7 @@
       </c>
       <c r="K39" s="33"/>
     </row>
-    <row r="40" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
         <v>47</v>
       </c>
@@ -2463,7 +2466,7 @@
       </c>
       <c r="K40" s="33"/>
     </row>
-    <row r="41" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
         <v>48</v>
       </c>
@@ -2496,7 +2499,7 @@
       </c>
       <c r="K41" s="33"/>
     </row>
-    <row r="42" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
         <v>49</v>
       </c>
@@ -2529,7 +2532,7 @@
       </c>
       <c r="K42" s="33"/>
     </row>
-    <row r="43" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
         <v>50</v>
       </c>
@@ -2562,7 +2565,7 @@
       </c>
       <c r="K43" s="33"/>
     </row>
-    <row r="44" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="9" t="s">
         <v>51</v>
       </c>
@@ -2595,7 +2598,7 @@
       </c>
       <c r="K44" s="33"/>
     </row>
-    <row r="45" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
         <v>52</v>
       </c>
@@ -2628,7 +2631,7 @@
       </c>
       <c r="K45" s="33"/>
     </row>
-    <row r="46" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
         <v>53</v>
       </c>
@@ -2661,7 +2664,7 @@
       </c>
       <c r="K46" s="33"/>
     </row>
-    <row r="47" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
         <v>54</v>
       </c>
@@ -2694,7 +2697,7 @@
       </c>
       <c r="K47" s="33"/>
     </row>
-    <row r="48" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
         <v>55</v>
       </c>
@@ -2727,7 +2730,7 @@
       </c>
       <c r="K48" s="33"/>
     </row>
-    <row r="49" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
         <v>56</v>
       </c>
@@ -2760,7 +2763,7 @@
       </c>
       <c r="K49" s="33"/>
     </row>
-    <row r="50" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="30" t="s">
         <v>57</v>
       </c>
@@ -2793,7 +2796,7 @@
       </c>
       <c r="K50" s="34"/>
     </row>
-    <row r="51" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="31" t="s">
         <v>58</v>
       </c>
@@ -2826,7 +2829,7 @@
       </c>
       <c r="K51" s="35"/>
     </row>
-    <row r="52" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="8" t="s">
         <v>59</v>
       </c>
@@ -2861,7 +2864,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
         <v>60</v>
       </c>
@@ -2896,7 +2899,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="9" t="s">
         <v>61</v>
       </c>
@@ -2931,7 +2934,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="s">
         <v>62</v>
       </c>
@@ -2966,7 +2969,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
         <v>63</v>
       </c>
@@ -3001,7 +3004,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
         <v>64</v>
       </c>
@@ -3036,7 +3039,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="s">
         <v>92</v>
       </c>
@@ -3071,7 +3074,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
         <v>93</v>
       </c>
@@ -3106,7 +3109,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="9" t="s">
         <v>94</v>
       </c>
@@ -3141,7 +3144,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
         <v>95</v>
       </c>
@@ -3176,41 +3179,69 @@
         <v>108</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
+      <c r="B62" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="D62" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
-      <c r="J62" s="20"/>
-      <c r="K62" s="33"/>
-    </row>
-    <row r="63" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E62" s="2">
+        <v>500</v>
+      </c>
+      <c r="F62" s="2">
+        <v>200</v>
+      </c>
+      <c r="G62" s="2">
+        <v>30</v>
+      </c>
+      <c r="H62" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="I62" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="J62" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="K62" s="33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
+      <c r="B63" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="D63" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
+      <c r="E63" s="2">
+        <v>500</v>
+      </c>
+      <c r="F63" s="2">
+        <v>200</v>
+      </c>
+      <c r="G63" s="2">
+        <v>30</v>
+      </c>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
       <c r="J63" s="20"/>
       <c r="K63" s="33"/>
     </row>
-    <row r="64" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="9"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -3223,7 +3254,7 @@
       <c r="J64" s="20"/>
       <c r="K64" s="33"/>
     </row>
-    <row r="65" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="9"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -3236,7 +3267,7 @@
       <c r="J65" s="20"/>
       <c r="K65" s="33"/>
     </row>
-    <row r="66" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -3249,7 +3280,7 @@
       <c r="J66" s="20"/>
       <c r="K66" s="33"/>
     </row>
-    <row r="67" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="9"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -3262,7 +3293,7 @@
       <c r="J67" s="20"/>
       <c r="K67" s="33"/>
     </row>
-    <row r="68" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="9"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -3275,7 +3306,7 @@
       <c r="J68" s="20"/>
       <c r="K68" s="33"/>
     </row>
-    <row r="69" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="9"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -3288,7 +3319,7 @@
       <c r="J69" s="20"/>
       <c r="K69" s="33"/>
     </row>
-    <row r="70" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="9"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -3301,7 +3332,7 @@
       <c r="J70" s="20"/>
       <c r="K70" s="33"/>
     </row>
-    <row r="71" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="9"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -3314,7 +3345,7 @@
       <c r="J71" s="20"/>
       <c r="K71" s="33"/>
     </row>
-    <row r="72" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="9"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -3327,7 +3358,7 @@
       <c r="J72" s="20"/>
       <c r="K72" s="33"/>
     </row>
-    <row r="73" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="9"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -3340,7 +3371,7 @@
       <c r="J73" s="20"/>
       <c r="K73" s="33"/>
     </row>
-    <row r="74" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="9"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -3353,7 +3384,7 @@
       <c r="J74" s="20"/>
       <c r="K74" s="33"/>
     </row>
-    <row r="75" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="9"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -3366,7 +3397,7 @@
       <c r="J75" s="20"/>
       <c r="K75" s="33"/>
     </row>
-    <row r="76" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="9"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -3379,7 +3410,7 @@
       <c r="J76" s="20"/>
       <c r="K76" s="33"/>
     </row>
-    <row r="77" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="9"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -3392,7 +3423,7 @@
       <c r="J77" s="20"/>
       <c r="K77" s="33"/>
     </row>
-    <row r="78" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="9"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -3405,7 +3436,7 @@
       <c r="J78" s="20"/>
       <c r="K78" s="33"/>
     </row>
-    <row r="79" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="9"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -3418,7 +3449,7 @@
       <c r="J79" s="20"/>
       <c r="K79" s="33"/>
     </row>
-    <row r="80" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="9"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -3431,7 +3462,7 @@
       <c r="J80" s="20"/>
       <c r="K80" s="33"/>
     </row>
-    <row r="81" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="9"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -3444,7 +3475,7 @@
       <c r="J81" s="20"/>
       <c r="K81" s="33"/>
     </row>
-    <row r="82" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="9"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -3457,7 +3488,7 @@
       <c r="J82" s="20"/>
       <c r="K82" s="33"/>
     </row>
-    <row r="83" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="9"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -3470,7 +3501,7 @@
       <c r="J83" s="20"/>
       <c r="K83" s="33"/>
     </row>
-    <row r="84" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="9"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -3483,7 +3514,7 @@
       <c r="J84" s="20"/>
       <c r="K84" s="33"/>
     </row>
-    <row r="85" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="9"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -3496,7 +3527,7 @@
       <c r="J85" s="20"/>
       <c r="K85" s="33"/>
     </row>
-    <row r="86" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="9"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -3509,7 +3540,7 @@
       <c r="J86" s="20"/>
       <c r="K86" s="33"/>
     </row>
-    <row r="87" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="9"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -3522,7 +3553,7 @@
       <c r="J87" s="20"/>
       <c r="K87" s="33"/>
     </row>
-    <row r="88" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="9"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -3535,7 +3566,7 @@
       <c r="J88" s="20"/>
       <c r="K88" s="33"/>
     </row>
-    <row r="89" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="9"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -3548,7 +3579,7 @@
       <c r="J89" s="20"/>
       <c r="K89" s="33"/>
     </row>
-    <row r="90" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="9"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -3561,7 +3592,7 @@
       <c r="J90" s="20"/>
       <c r="K90" s="33"/>
     </row>
-    <row r="91" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="9"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -3574,7 +3605,7 @@
       <c r="J91" s="20"/>
       <c r="K91" s="33"/>
     </row>
-    <row r="92" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="9"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -3587,7 +3618,7 @@
       <c r="J92" s="20"/>
       <c r="K92" s="33"/>
     </row>
-    <row r="93" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="9"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -3600,7 +3631,7 @@
       <c r="J93" s="20"/>
       <c r="K93" s="33"/>
     </row>
-    <row r="94" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="9"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -3613,7 +3644,7 @@
       <c r="J94" s="20"/>
       <c r="K94" s="33"/>
     </row>
-    <row r="95" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="9"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -3626,7 +3657,7 @@
       <c r="J95" s="20"/>
       <c r="K95" s="33"/>
     </row>
-    <row r="96" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="9"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -3639,7 +3670,7 @@
       <c r="J96" s="20"/>
       <c r="K96" s="33"/>
     </row>
-    <row r="97" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="9"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -3652,7 +3683,7 @@
       <c r="J97" s="20"/>
       <c r="K97" s="33"/>
     </row>
-    <row r="98" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="9"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -3665,7 +3696,7 @@
       <c r="J98" s="20"/>
       <c r="K98" s="33"/>
     </row>
-    <row r="99" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="9"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -3678,7 +3709,7 @@
       <c r="J99" s="20"/>
       <c r="K99" s="33"/>
     </row>
-    <row r="100" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="9"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -3691,7 +3722,7 @@
       <c r="J100" s="20"/>
       <c r="K100" s="33"/>
     </row>
-    <row r="101" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="9"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -3704,7 +3735,7 @@
       <c r="J101" s="20"/>
       <c r="K101" s="33"/>
     </row>
-    <row r="102" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="9"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -3717,7 +3748,7 @@
       <c r="J102" s="20"/>
       <c r="K102" s="33"/>
     </row>
-    <row r="103" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="9"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -3730,7 +3761,7 @@
       <c r="J103" s="20"/>
       <c r="K103" s="33"/>
     </row>
-    <row r="104" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="9"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -3743,7 +3774,7 @@
       <c r="J104" s="20"/>
       <c r="K104" s="33"/>
     </row>
-    <row r="105" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="9"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -3756,7 +3787,7 @@
       <c r="J105" s="20"/>
       <c r="K105" s="33"/>
     </row>
-    <row r="106" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="9"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -3769,7 +3800,7 @@
       <c r="J106" s="20"/>
       <c r="K106" s="33"/>
     </row>
-    <row r="107" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="9"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -3782,7 +3813,7 @@
       <c r="J107" s="20"/>
       <c r="K107" s="33"/>
     </row>
-    <row r="108" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="9"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -3795,7 +3826,7 @@
       <c r="J108" s="20"/>
       <c r="K108" s="33"/>
     </row>
-    <row r="109" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="9"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -3808,7 +3839,7 @@
       <c r="J109" s="20"/>
       <c r="K109" s="33"/>
     </row>
-    <row r="110" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="9"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -3821,7 +3852,7 @@
       <c r="J110" s="20"/>
       <c r="K110" s="33"/>
     </row>
-    <row r="111" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="9"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -3834,7 +3865,7 @@
       <c r="J111" s="20"/>
       <c r="K111" s="33"/>
     </row>
-    <row r="112" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="9"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -3847,7 +3878,7 @@
       <c r="J112" s="20"/>
       <c r="K112" s="33"/>
     </row>
-    <row r="113" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="9"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -3860,7 +3891,7 @@
       <c r="J113" s="20"/>
       <c r="K113" s="33"/>
     </row>
-    <row r="114" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="9"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -3873,7 +3904,7 @@
       <c r="J114" s="20"/>
       <c r="K114" s="33"/>
     </row>
-    <row r="115" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="9"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -3886,7 +3917,7 @@
       <c r="J115" s="20"/>
       <c r="K115" s="33"/>
     </row>
-    <row r="116" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="9"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -3899,7 +3930,7 @@
       <c r="J116" s="20"/>
       <c r="K116" s="33"/>
     </row>
-    <row r="117" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="9"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -3912,7 +3943,7 @@
       <c r="J117" s="20"/>
       <c r="K117" s="33"/>
     </row>
-    <row r="118" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="9"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -3925,7 +3956,7 @@
       <c r="J118" s="20"/>
       <c r="K118" s="33"/>
     </row>
-    <row r="119" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="9"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -3938,7 +3969,7 @@
       <c r="J119" s="20"/>
       <c r="K119" s="33"/>
     </row>
-    <row r="120" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="9"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -3951,7 +3982,7 @@
       <c r="J120" s="20"/>
       <c r="K120" s="33"/>
     </row>
-    <row r="121" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="9"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -3964,7 +3995,7 @@
       <c r="J121" s="20"/>
       <c r="K121" s="33"/>
     </row>
-    <row r="122" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="9"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -3977,7 +4008,7 @@
       <c r="J122" s="20"/>
       <c r="K122" s="33"/>
     </row>
-    <row r="123" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="9"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -3990,7 +4021,7 @@
       <c r="J123" s="20"/>
       <c r="K123" s="33"/>
     </row>
-    <row r="124" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="9"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -4003,7 +4034,7 @@
       <c r="J124" s="20"/>
       <c r="K124" s="33"/>
     </row>
-    <row r="125" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="9"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -4016,7 +4047,7 @@
       <c r="J125" s="20"/>
       <c r="K125" s="33"/>
     </row>
-    <row r="126" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="9"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -4029,7 +4060,7 @@
       <c r="J126" s="20"/>
       <c r="K126" s="33"/>
     </row>
-    <row r="127" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="9"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -4042,7 +4073,7 @@
       <c r="J127" s="20"/>
       <c r="K127" s="33"/>
     </row>
-    <row r="128" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="9"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -4055,7 +4086,7 @@
       <c r="J128" s="20"/>
       <c r="K128" s="33"/>
     </row>
-    <row r="129" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="9"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -4068,7 +4099,7 @@
       <c r="J129" s="20"/>
       <c r="K129" s="33"/>
     </row>
-    <row r="130" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="9"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -4081,7 +4112,7 @@
       <c r="J130" s="20"/>
       <c r="K130" s="33"/>
     </row>
-    <row r="131" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="9"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -4094,7 +4125,7 @@
       <c r="J131" s="20"/>
       <c r="K131" s="33"/>
     </row>
-    <row r="132" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="9"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -4107,7 +4138,7 @@
       <c r="J132" s="20"/>
       <c r="K132" s="33"/>
     </row>
-    <row r="133" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="9"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -4120,7 +4151,7 @@
       <c r="J133" s="20"/>
       <c r="K133" s="33"/>
     </row>
-    <row r="134" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" s="9"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -4133,7 +4164,7 @@
       <c r="J134" s="20"/>
       <c r="K134" s="33"/>
     </row>
-    <row r="135" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" s="9"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -4146,7 +4177,7 @@
       <c r="J135" s="20"/>
       <c r="K135" s="33"/>
     </row>
-    <row r="136" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" s="9"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -4159,7 +4190,7 @@
       <c r="J136" s="20"/>
       <c r="K136" s="33"/>
     </row>
-    <row r="137" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="9"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -4172,7 +4203,7 @@
       <c r="J137" s="20"/>
       <c r="K137" s="33"/>
     </row>
-    <row r="138" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="9"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -4185,7 +4216,7 @@
       <c r="J138" s="20"/>
       <c r="K138" s="33"/>
     </row>
-    <row r="139" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="9"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -4198,7 +4229,7 @@
       <c r="J139" s="20"/>
       <c r="K139" s="33"/>
     </row>
-    <row r="140" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A140" s="10"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
@@ -4211,28 +4242,28 @@
       <c r="J140" s="21"/>
       <c r="K140" s="36"/>
     </row>
-    <row r="141" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="142" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="143" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="144" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="145" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="146" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="147" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="148" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="149" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="150" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="151" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="152" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="153" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="154" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="155" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="156" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="157" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="158" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="160" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="161" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="162" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="142" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="143" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="144" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="145" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="146" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="147" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="148" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="149" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="150" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="151" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="152" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="153" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="154" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="155" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="156" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="157" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="158" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="159" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="160" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="161" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="162" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>